<commit_message>
Actualizacion del analisis economico
</commit_message>
<xml_diff>
--- a/4 - Evaluación Económica del Proyecto/Analisis_economico.xlsx
+++ b/4 - Evaluación Económica del Proyecto/Analisis_economico.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Repositories\SediaAutomatica\4 - Evaluación Económica del Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yeison\Documents\GitHub\SediaAutomatica\4 - Evaluación Económica del Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F68A26A-C850-4D3C-9372-5665169E5C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38B7564-FCC9-488E-A737-550B9F97CE8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="76">
   <si>
     <t>Insumos necesarios</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>Maquina de inyeccion de plastico</t>
-  </si>
-  <si>
-    <t>Maquina de doblado</t>
   </si>
   <si>
     <t>Robot ABB para soldado</t>
@@ -332,12 +329,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]\([$$-240A]#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="[$$-240A]#,##0;[Red]\([$$-240A]#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="[$$-240A]#,##0.00;[Red]\([$$-240A]#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="[$$-240A]#,##0;[Red]\([$$-240A]#,##0\)"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -910,12 +907,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -932,8 +929,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
@@ -943,13 +940,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -962,35 +959,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="17" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1004,20 +1001,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="33" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="34" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="34" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="35" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="33" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="34" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="35" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1025,16 +1022,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
-    <cellStyle name="Millares" xfId="3" builtinId="3"/>
-    <cellStyle name="Moneda" xfId="4" builtinId="4"/>
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
+    <cellStyle name="Currency" xfId="4" builtinId="4"/>
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="5" builtinId="5"/>
-    <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]\([$$-240A]#,##0.00\)"/>
+      <numFmt numFmtId="165" formatCode="[$$-240A]#,##0.00;[Red]\([$$-240A]#,##0.00\)"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1087,7 +1084,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]\([$$-240A]#,##0.00\)"/>
+      <numFmt numFmtId="165" formatCode="[$$-240A]#,##0.00;[Red]\([$$-240A]#,##0.00\)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1128,7 +1125,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="[$$-240A]#,##0.00;[Red]\([$$-240A]#,##0.00\)"/>
+      <numFmt numFmtId="165" formatCode="[$$-240A]#,##0.00;[Red]\([$$-240A]#,##0.00\)"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1351,7 +1348,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1649,11 +1646,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="69.5703125" bestFit="1" customWidth="1"/>
@@ -1837,7 +1834,7 @@
         <v>59</v>
       </c>
       <c r="C14" s="78">
-        <v>850</v>
+        <v>700</v>
       </c>
       <c r="F14" s="5"/>
       <c r="H14" s="62">
@@ -1847,20 +1844,20 @@
     </row>
     <row r="15" spans="2:9" ht="13.5" thickBot="1">
       <c r="B15" s="77" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="78">
         <v>15</v>
       </c>
       <c r="D15" s="80" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="6"/>
     </row>
     <row r="16" spans="2:9" ht="13.5" thickBot="1">
       <c r="B16" s="76" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C16" s="79">
         <v>500</v>
@@ -2127,32 +2124,30 @@
       <c r="B26" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="68">
-        <v>-15000</v>
-      </c>
+      <c r="C26" s="68"/>
       <c r="D26" s="68"/>
       <c r="E26" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F26" s="60">
         <f t="shared" si="1"/>
-        <v>-60000000</v>
+        <v>0</v>
       </c>
       <c r="G26" s="55">
         <f t="shared" si="2"/>
-        <v>-60000000</v>
+        <v>0</v>
       </c>
       <c r="H26" s="33">
         <f t="shared" si="3"/>
-        <v>-48000000</v>
+        <v>0</v>
       </c>
       <c r="I26" s="33">
         <f>Tabelle1[[#This Row],[Precio ]]</f>
-        <v>-60000000</v>
+        <v>0</v>
       </c>
       <c r="J26" s="33">
         <f t="shared" si="4"/>
-        <v>-66000000.000000007</v>
+        <v>0</v>
       </c>
       <c r="K26" s="33"/>
       <c r="L26" s="40"/>
@@ -2240,7 +2235,7 @@
       </c>
       <c r="C29" s="68">
         <f>C14*G12*C1</f>
-        <v>17850</v>
+        <v>14700</v>
       </c>
       <c r="D29" s="68"/>
       <c r="E29" s="8" t="s">
@@ -2248,23 +2243,23 @@
       </c>
       <c r="F29" s="60">
         <f t="shared" si="1"/>
-        <v>71400000</v>
+        <v>58800000</v>
       </c>
       <c r="G29" s="55">
         <f t="shared" si="2"/>
-        <v>71400000</v>
+        <v>58800000</v>
       </c>
       <c r="H29" s="33">
         <f>I29*1.2</f>
-        <v>85680000</v>
+        <v>70560000</v>
       </c>
       <c r="I29" s="33">
         <f>Tabelle1[[#This Row],[Precio ]]</f>
-        <v>71400000</v>
+        <v>58800000</v>
       </c>
       <c r="J29" s="33">
         <f>I29*(1-0.1)</f>
-        <v>64260000</v>
+        <v>52920000</v>
       </c>
       <c r="K29" s="33"/>
       <c r="L29" s="40"/>
@@ -2278,7 +2273,7 @@
       </c>
       <c r="C30" s="68">
         <f>C14*I12*C2</f>
-        <v>15300</v>
+        <v>12600</v>
       </c>
       <c r="D30" s="68"/>
       <c r="E30" s="8" t="s">
@@ -2286,23 +2281,23 @@
       </c>
       <c r="F30" s="60">
         <f t="shared" si="1"/>
-        <v>61200000</v>
+        <v>50400000</v>
       </c>
       <c r="G30" s="55">
         <f t="shared" si="2"/>
-        <v>61200000</v>
+        <v>50400000</v>
       </c>
       <c r="H30" s="33">
         <f>I30*1.2</f>
-        <v>73440000</v>
+        <v>60480000</v>
       </c>
       <c r="I30" s="33">
         <f>Tabelle1[[#This Row],[Precio ]]</f>
-        <v>61200000</v>
+        <v>50400000</v>
       </c>
       <c r="J30" s="33">
         <f>I30*(1-0.1)</f>
-        <v>55080000</v>
+        <v>45360000</v>
       </c>
       <c r="K30" s="33"/>
       <c r="L30" s="40"/>
@@ -2497,35 +2492,31 @@
       <c r="A36" s="55">
         <v>16</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="68">
-        <v>-5000</v>
-      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="68"/>
       <c r="D36" s="68"/>
       <c r="E36" s="8" t="s">
         <v>5</v>
       </c>
       <c r="F36" s="60">
         <f t="shared" si="1"/>
-        <v>-20000000</v>
+        <v>0</v>
       </c>
       <c r="G36" s="55">
         <f t="shared" si="2"/>
-        <v>-20000000</v>
+        <v>0</v>
       </c>
       <c r="H36" s="33">
         <f t="shared" si="3"/>
-        <v>-16000000</v>
+        <v>0</v>
       </c>
       <c r="I36" s="33">
         <f>Tabelle1[[#This Row],[Precio ]]</f>
-        <v>-20000000</v>
+        <v>0</v>
       </c>
       <c r="J36" s="33">
         <f t="shared" si="4"/>
-        <v>-22000000</v>
+        <v>0</v>
       </c>
       <c r="K36" s="33"/>
       <c r="L36" s="40"/>
@@ -2535,7 +2526,7 @@
         <v>17</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="68">
         <v>-20000</v>
@@ -2572,7 +2563,7 @@
         <v>18</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" s="68">
         <v>-20000</v>
@@ -2609,7 +2600,7 @@
         <v>19</v>
       </c>
       <c r="B39" s="63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C39" s="68">
         <f>-15000*C15</f>
@@ -2647,7 +2638,7 @@
         <v>20</v>
       </c>
       <c r="B40" s="63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C40" s="68">
         <v>-750</v>
@@ -2684,7 +2675,7 @@
         <v>21</v>
       </c>
       <c r="B41" s="63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C41" s="68">
         <v>-1400</v>
@@ -2721,7 +2712,7 @@
         <v>22</v>
       </c>
       <c r="B42" s="63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C42" s="68">
         <v>-60</v>
@@ -2758,7 +2749,7 @@
         <v>23</v>
       </c>
       <c r="B43" s="63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="68">
         <f>-500*D16*0.5</f>
@@ -2796,7 +2787,7 @@
         <v>24</v>
       </c>
       <c r="B44" s="63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="68">
         <f>-350*D16*0.5</f>
@@ -2834,7 +2825,7 @@
         <v>25</v>
       </c>
       <c r="B45" s="64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C45" s="68"/>
       <c r="D45" s="68">
@@ -2871,7 +2862,7 @@
         <v>26</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C46" s="68">
         <f>-1500*C15</f>
@@ -3174,10 +3165,10 @@
       </c>
       <c r="H59" s="81">
         <f ca="1">Balance!G3</f>
-        <v>1655498550.1058669</v>
+        <v>70602991.871020079</v>
       </c>
       <c r="I59" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -3188,7 +3179,7 @@
       </c>
       <c r="H60" s="82">
         <f t="dataTable" ref="H60:H64" dt2D="0" dtr="0" r1="G19" ca="1"/>
-        <v>4684483507.8246927</v>
+        <v>2612873087.1198092</v>
       </c>
       <c r="I60" s="86">
         <v>0.2</v>
@@ -3201,7 +3192,7 @@
         <v>2</v>
       </c>
       <c r="H61" s="83">
-        <v>1655498550.1058669</v>
+        <v>70602991.871020079</v>
       </c>
       <c r="I61" s="86">
         <v>0.5</v>
@@ -3214,7 +3205,7 @@
         <v>3</v>
       </c>
       <c r="H62" s="83">
-        <v>141006071.24645495</v>
+        <v>-1200532055.7533746</v>
       </c>
       <c r="I62" s="86">
         <v>0.3</v>
@@ -3231,7 +3222,7 @@
       </c>
       <c r="I63" s="88">
         <f>H60*I60+H61*I61+H62*I62</f>
-        <v>1806947797.9918084</v>
+        <v>197716496.63345957</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="13.5" thickBot="1">
@@ -3267,11 +3258,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S182"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:S1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="11.5703125"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
@@ -3323,15 +3314,15 @@
       </c>
       <c r="B2" s="42">
         <f>IF(A2=0,$N$42,0)</f>
-        <v>-1726659000</v>
+        <v>-1646659000</v>
       </c>
       <c r="C2" s="42">
         <f t="shared" ref="C2:C33" si="0">-PV($K$1,A2,,B2)</f>
-        <v>-1726659000</v>
+        <v>-1646659000</v>
       </c>
       <c r="D2" s="42">
         <f>SUM($C$2:C2)</f>
-        <v>-1726659000</v>
+        <v>-1646659000</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="8" t="s">
@@ -3355,16 +3346,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="42">
-        <f t="shared" ref="B3:B34" si="1">IF(A3=0,$N$42,0)+IF(A3=0,0,$O$42)+IF(MOD(A3,2)=0,$P$42,0)+IF(MOD(A3,3)=0,$Q$42,0)+IF(MOD(A3,6)=0,$R$42,0)+IF(MOD(A3,12)=0,$S$42,0)</f>
-        <v>62500000</v>
+        <v>0</v>
       </c>
       <c r="C3" s="42">
         <f t="shared" si="0"/>
-        <v>62344139.650872819</v>
+        <v>0</v>
       </c>
       <c r="D3" s="42">
         <f>SUM($C$2:C3)</f>
-        <v>-1664314860.3491273</v>
+        <v>-1646659000</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="8" t="s">
@@ -3372,7 +3362,7 @@
       </c>
       <c r="G3" s="42">
         <f ca="1">NPV(K4,OFFSET(C3,0,0,MATCH(G2*12,A3:A182,0),1))+D2</f>
-        <v>1655498550.1058669</v>
+        <v>70602991.871020079</v>
       </c>
       <c r="J3" s="45" t="s">
         <v>27</v>
@@ -3386,16 +3376,15 @@
         <v>2</v>
       </c>
       <c r="B4" s="42">
-        <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="42">
         <f t="shared" si="0"/>
-        <v>62188667.980920523</v>
+        <v>0</v>
       </c>
       <c r="D4" s="42">
         <f>SUM($C$2:C4)</f>
-        <v>-1602126192.3682067</v>
+        <v>-1646659000</v>
       </c>
       <c r="E4" s="1"/>
       <c r="J4" s="22" t="s">
@@ -3410,16 +3399,15 @@
         <v>3</v>
       </c>
       <c r="B5" s="42">
-        <f t="shared" si="1"/>
-        <v>56140000</v>
+        <v>0</v>
       </c>
       <c r="C5" s="42">
         <f t="shared" si="0"/>
-        <v>55721046.510904796</v>
+        <v>0</v>
       </c>
       <c r="D5" s="42">
         <f>SUM($C$2:C5)</f>
-        <v>-1546405145.857302</v>
+        <v>-1646659000</v>
       </c>
       <c r="E5" s="1"/>
       <c r="G5" s="29"/>
@@ -3429,16 +3417,15 @@
         <v>4</v>
       </c>
       <c r="B6" s="42">
-        <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>0</v>
       </c>
       <c r="C6" s="42">
         <f t="shared" si="0"/>
-        <v>61878886.803858712</v>
+        <v>0</v>
       </c>
       <c r="D6" s="42">
         <f>SUM($C$2:C6)</f>
-        <v>-1484526259.0534432</v>
+        <v>-1646659000</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -3447,16 +3434,15 @@
         <v>5</v>
       </c>
       <c r="B7" s="42">
-        <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>0</v>
       </c>
       <c r="C7" s="42">
         <f t="shared" si="0"/>
-        <v>61724575.3654451</v>
+        <v>0</v>
       </c>
       <c r="D7" s="42">
         <f>SUM($C$2:C7)</f>
-        <v>-1422801683.6879981</v>
+        <v>-1646659000</v>
       </c>
       <c r="E7" s="1"/>
       <c r="M7" t="s">
@@ -3486,16 +3472,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="42">
-        <f t="shared" si="1"/>
-        <v>56140000</v>
+        <f t="shared" ref="B3:B34" si="1">IF(A8=0,$N$42,0)+IF(A8=0,0,$O$42)+IF(MOD(A8,2)=0,$P$42,0)+IF(MOD(A8,3)=0,$Q$42,0)+IF(MOD(A8,6)=0,$R$42,0)+IF(MOD(A8,12)=0,$S$42,0)</f>
+        <v>32740000</v>
       </c>
       <c r="C8" s="42">
         <f t="shared" si="0"/>
-        <v>55305219.527438819</v>
+        <v>32253168.637840167</v>
       </c>
       <c r="D8" s="42">
         <f>SUM($C$2:C8)</f>
-        <v>-1367496464.1605592</v>
+        <v>-1614405831.3621597</v>
       </c>
       <c r="E8" s="1"/>
       <c r="M8">
@@ -3532,15 +3518,15 @@
       </c>
       <c r="B9" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C9" s="42">
         <f t="shared" si="0"/>
-        <v>61417105.978639551</v>
+        <v>38422541.500236899</v>
       </c>
       <c r="D9" s="42">
         <f>SUM($C$2:C9)</f>
-        <v>-1306079358.1819196</v>
+        <v>-1575983289.8619227</v>
       </c>
       <c r="E9" s="1"/>
       <c r="G9" s="29"/>
@@ -3578,15 +3564,15 @@
       </c>
       <c r="B10" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C10" s="42">
         <f t="shared" si="0"/>
-        <v>61263946.113356158</v>
+        <v>38326724.688515611</v>
       </c>
       <c r="D10" s="42">
         <f>SUM($C$2:C10)</f>
-        <v>-1244815412.0685635</v>
+        <v>-1537656565.1734071</v>
       </c>
       <c r="E10" s="1"/>
       <c r="M10">
@@ -3623,15 +3609,15 @@
       </c>
       <c r="B11" s="42">
         <f t="shared" si="1"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C11" s="42">
         <f t="shared" si="0"/>
-        <v>54892495.717567116</v>
+        <v>32012474.3461551</v>
       </c>
       <c r="D11" s="42">
         <f>SUM($C$2:C11)</f>
-        <v>-1189922916.3509963</v>
+        <v>-1505644090.8272519</v>
       </c>
       <c r="E11" s="1"/>
       <c r="M11">
@@ -3668,15 +3654,15 @@
       </c>
       <c r="B12" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C12" s="42">
         <f t="shared" si="0"/>
-        <v>60958771.2647122</v>
+        <v>38135807.303203948</v>
       </c>
       <c r="D12" s="42">
         <f>SUM($C$2:C12)</f>
-        <v>-1128964145.0862842</v>
+        <v>-1467508283.5240479</v>
       </c>
       <c r="E12" s="1"/>
       <c r="M12">
@@ -3713,15 +3699,15 @@
       </c>
       <c r="B13" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C13" s="42">
         <f t="shared" si="0"/>
-        <v>60806754.378765292</v>
+        <v>38040705.539355569</v>
       </c>
       <c r="D13" s="42">
         <f>SUM($C$2:C13)</f>
-        <v>-1068157390.7075188</v>
+        <v>-1429467577.9846923</v>
       </c>
       <c r="E13" s="1"/>
       <c r="M13">
@@ -3729,7 +3715,7 @@
       </c>
       <c r="N13" s="1">
         <f>IF(Costos!E26= $N$7, Costos!G26,0)</f>
-        <v>-60000000</v>
+        <v>0</v>
       </c>
       <c r="O13" s="1">
         <f>IF(Costos!E26= $O$7, Costos!G26,0)</f>
@@ -3758,15 +3744,15 @@
       </c>
       <c r="B14" s="42">
         <f t="shared" si="1"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C14" s="42">
         <f t="shared" si="0"/>
-        <v>-32860515.962334048</v>
+        <v>-55569791.612618059</v>
       </c>
       <c r="D14" s="42">
         <f>SUM($C$2:C14)</f>
-        <v>-1101017906.669853</v>
+        <v>-1485037369.5973103</v>
       </c>
       <c r="E14" s="1"/>
       <c r="M14">
@@ -3803,15 +3789,15 @@
       </c>
       <c r="B15" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C15" s="42">
         <f t="shared" si="0"/>
-        <v>60503856.944934703</v>
+        <v>37851212.904751152</v>
       </c>
       <c r="D15" s="42">
         <f>SUM($C$2:C15)</f>
-        <v>-1040514049.7249182</v>
+        <v>-1447186156.6925592</v>
       </c>
       <c r="E15" s="1"/>
       <c r="M15">
@@ -3848,15 +3834,15 @@
       </c>
       <c r="B16" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C16" s="42">
         <f t="shared" si="0"/>
-        <v>60352974.508663066</v>
+        <v>37756820.852619611</v>
       </c>
       <c r="D16" s="42">
         <f>SUM($C$2:C16)</f>
-        <v>-980161075.21625519</v>
+        <v>-1409429335.8399396</v>
       </c>
       <c r="E16" s="1"/>
       <c r="M16">
@@ -3868,7 +3854,7 @@
       </c>
       <c r="O16" s="1">
         <f>IF(Costos!E29= $O$7, Costos!G29,0)</f>
-        <v>71400000</v>
+        <v>58800000</v>
       </c>
       <c r="P16" s="1">
         <f>IF(Costos!E29= $P$7, Costos!G29,0)</f>
@@ -3893,15 +3879,15 @@
       </c>
       <c r="B17" s="42">
         <f t="shared" si="1"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C17" s="42">
         <f t="shared" si="0"/>
-        <v>54076265.159762107</v>
+        <v>31536461.014082853</v>
       </c>
       <c r="D17" s="42">
         <f>SUM($C$2:C17)</f>
-        <v>-926084810.05649304</v>
+        <v>-1377892874.8258567</v>
       </c>
       <c r="E17" s="1"/>
       <c r="M17">
@@ -3913,7 +3899,7 @@
       </c>
       <c r="O17" s="1">
         <f>IF(Costos!E30= $O$7, Costos!G30,0)</f>
-        <v>61200000</v>
+        <v>50400000</v>
       </c>
       <c r="P17" s="1">
         <f>IF(Costos!E30= $P$7, Costos!G30,0)</f>
@@ -3938,15 +3924,15 @@
       </c>
       <c r="B18" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C18" s="42">
         <f t="shared" si="0"/>
-        <v>60052337.494083308</v>
+        <v>37568742.336298518</v>
       </c>
       <c r="D18" s="42">
         <f>SUM($C$2:C18)</f>
-        <v>-866032472.56240976</v>
+        <v>-1340324132.4895582</v>
       </c>
       <c r="E18" s="1"/>
       <c r="M18">
@@ -3983,15 +3969,15 @@
       </c>
       <c r="B19" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C19" s="42">
         <f t="shared" si="0"/>
-        <v>59902581.041479617</v>
+        <v>37475054.699549645</v>
       </c>
       <c r="D19" s="42">
         <f>SUM($C$2:C19)</f>
-        <v>-806129891.52093017</v>
+        <v>-1302849077.7900085</v>
       </c>
       <c r="E19" s="1"/>
       <c r="M19">
@@ -4028,15 +4014,15 @@
       </c>
       <c r="B20" s="42">
         <f t="shared" si="1"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C20" s="42">
         <f t="shared" si="0"/>
-        <v>53672712.613165729</v>
+        <v>31301115.264607161</v>
       </c>
       <c r="D20" s="42">
         <f>SUM($C$2:C20)</f>
-        <v>-752457178.90776443</v>
+        <v>-1271547962.5254014</v>
       </c>
       <c r="E20" s="1"/>
       <c r="M20">
@@ -4073,15 +4059,15 @@
       </c>
       <c r="B21" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C21" s="42">
         <f t="shared" si="0"/>
-        <v>59604187.57742016</v>
+        <v>37288379.748434052</v>
       </c>
       <c r="D21" s="42">
         <f>SUM($C$2:C21)</f>
-        <v>-692852991.33034432</v>
+        <v>-1234259582.7769673</v>
       </c>
       <c r="E21" s="1"/>
       <c r="M21">
@@ -4118,15 +4104,15 @@
       </c>
       <c r="B22" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C22" s="42">
         <f t="shared" si="0"/>
-        <v>59455548.705656014</v>
+        <v>37195391.270258404</v>
       </c>
       <c r="D22" s="42">
         <f>SUM($C$2:C22)</f>
-        <v>-633397442.62468827</v>
+        <v>-1197064191.5067089</v>
       </c>
       <c r="E22" s="1"/>
       <c r="M22">
@@ -4163,15 +4149,15 @@
       </c>
       <c r="B23" s="42">
         <f t="shared" si="1"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C23" s="42">
         <f t="shared" si="0"/>
-        <v>53272171.640267797</v>
+        <v>31067525.819422293</v>
       </c>
       <c r="D23" s="42">
         <f>SUM($C$2:C23)</f>
-        <v>-580125270.98442042</v>
+        <v>-1165996665.6872866</v>
       </c>
       <c r="E23" s="1"/>
       <c r="M23">
@@ -4179,7 +4165,7 @@
       </c>
       <c r="N23" s="1">
         <f>IF(Costos!E36= $N$7, Costos!G36,0)</f>
-        <v>-20000000</v>
+        <v>0</v>
       </c>
       <c r="O23" s="1">
         <f>IF(Costos!E36= $O$7, Costos!G36,0)</f>
@@ -4208,15 +4194,15 @@
       </c>
       <c r="B24" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C24" s="42">
         <f t="shared" si="0"/>
-        <v>59159382.049271867</v>
+        <v>37010109.410024479</v>
       </c>
       <c r="D24" s="42">
         <f>SUM($C$2:C24)</f>
-        <v>-520965888.93514854</v>
+        <v>-1128986556.2772622</v>
       </c>
       <c r="E24" s="1"/>
       <c r="M24">
@@ -4253,15 +4239,15 @@
       </c>
       <c r="B25" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C25" s="42">
         <f t="shared" si="0"/>
-        <v>59011852.418226302</v>
+        <v>36917814.872842371</v>
       </c>
       <c r="D25" s="42">
         <f>SUM($C$2:C25)</f>
-        <v>-461954036.51692224</v>
+        <v>-1092068741.4044199</v>
       </c>
       <c r="E25" s="1"/>
       <c r="M25">
@@ -4298,15 +4284,15 @@
       </c>
       <c r="B26" s="42">
         <f t="shared" si="1"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C26" s="42">
         <f t="shared" si="0"/>
-        <v>-31890534.829025716</v>
+        <v>-53929475.023922406</v>
       </c>
       <c r="D26" s="42">
         <f>SUM($C$2:C26)</f>
-        <v>-493844571.34594798</v>
+        <v>-1145998216.4283423</v>
       </c>
       <c r="E26" s="1"/>
       <c r="M26">
@@ -4343,15 +4329,15 @@
       </c>
       <c r="B27" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C27" s="42">
         <f t="shared" si="0"/>
-        <v>58717895.951618508</v>
+        <v>36733915.707332537</v>
       </c>
       <c r="D27" s="42">
         <f>SUM($C$2:C27)</f>
-        <v>-435126675.39432949</v>
+        <v>-1109264300.7210097</v>
       </c>
       <c r="E27" s="1"/>
       <c r="M27">
@@ -4388,15 +4374,15 @@
       </c>
       <c r="B28" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C28" s="42">
         <f t="shared" si="0"/>
-        <v>58571467.283409983</v>
+        <v>36642309.932501286</v>
       </c>
       <c r="D28" s="42">
         <f>SUM($C$2:C28)</f>
-        <v>-376555208.11091948</v>
+        <v>-1072621990.7885084</v>
       </c>
       <c r="E28" s="1"/>
       <c r="M28">
@@ -4433,15 +4419,15 @@
       </c>
       <c r="B29" s="42">
         <f t="shared" si="1"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C29" s="42">
         <f t="shared" si="0"/>
-        <v>52480034.685935356</v>
+        <v>30605563.512959093</v>
       </c>
       <c r="D29" s="42">
         <f>SUM($C$2:C29)</f>
-        <v>-324075173.4249841</v>
+        <v>-1042016427.2755493</v>
       </c>
       <c r="E29" s="1"/>
       <c r="M29">
@@ -4478,15 +4464,15 @@
       </c>
       <c r="B30" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C30" s="42">
         <f t="shared" si="0"/>
-        <v>58279704.512693323</v>
+        <v>36459783.143140942</v>
       </c>
       <c r="D30" s="42">
         <f>SUM($C$2:C30)</f>
-        <v>-265795468.91229078</v>
+        <v>-1005556644.1324084</v>
       </c>
       <c r="E30" s="1"/>
       <c r="M30">
@@ -4523,15 +4509,15 @@
       </c>
       <c r="B31" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C31" s="42">
         <f t="shared" si="0"/>
-        <v>58134368.591215275</v>
+        <v>36368860.990664274</v>
       </c>
       <c r="D31" s="42">
         <f>SUM($C$2:C31)</f>
-        <v>-207661100.3210755</v>
+        <v>-969187783.14174414</v>
       </c>
       <c r="M31">
         <v>24</v>
@@ -4567,15 +4553,15 @@
       </c>
       <c r="B32" s="42">
         <f t="shared" si="1"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C32" s="42">
         <f t="shared" si="0"/>
-        <v>52088394.257728904</v>
+        <v>30377164.730994731</v>
       </c>
       <c r="D32" s="42">
         <f>SUM($C$2:C32)</f>
-        <v>-155572706.06334659</v>
+        <v>-938810618.41074944</v>
       </c>
       <c r="M32">
         <v>25</v>
@@ -4611,15 +4597,15 @@
       </c>
       <c r="B33" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C33" s="42">
         <f t="shared" si="0"/>
-        <v>57844783.145592675</v>
+        <v>36187696.335882775</v>
       </c>
       <c r="D33" s="42">
         <f>SUM($C$2:C33)</f>
-        <v>-97727922.91775392</v>
+        <v>-902622922.07486665</v>
       </c>
       <c r="M33">
         <v>26</v>
@@ -4655,15 +4641,15 @@
       </c>
       <c r="B34" s="42">
         <f t="shared" si="1"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C34" s="42">
         <f t="shared" ref="C34:C65" si="2">-PV($K$1,A34,,B34)</f>
-        <v>57700531.816052534</v>
+        <v>36097452.704122469</v>
       </c>
       <c r="D34" s="42">
         <f>SUM($C$2:C34)</f>
-        <v>-40027391.101701386</v>
+        <v>-866525469.37074423</v>
       </c>
       <c r="M34">
         <v>27</v>
@@ -4699,15 +4685,15 @@
       </c>
       <c r="B35" s="42">
         <f t="shared" ref="B35:B66" si="3">IF(A35=0,$N$42,0)+IF(A35=0,0,$O$42)+IF(MOD(A35,2)=0,$P$42,0)+IF(MOD(A35,3)=0,$Q$42,0)+IF(MOD(A35,6)=0,$R$42,0)+IF(MOD(A35,12)=0,$S$42,0)</f>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C35" s="42">
         <f t="shared" si="2"/>
-        <v>51699676.507183075</v>
+        <v>30150470.410494722</v>
       </c>
       <c r="D35" s="42">
         <f>SUM($C$2:C35)</f>
-        <v>11672285.405481689</v>
+        <v>-836374998.96024954</v>
       </c>
       <c r="M35">
         <v>28</v>
@@ -4743,15 +4729,15 @@
       </c>
       <c r="B36" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C36" s="42">
         <f t="shared" si="2"/>
-        <v>57413107.446896516</v>
+        <v>35917640.018778466</v>
       </c>
       <c r="D36" s="42">
         <f>SUM($C$2:C36)</f>
-        <v>69085392.852378204</v>
+        <v>-800457358.9414711</v>
       </c>
       <c r="M36">
         <v>29</v>
@@ -4787,15 +4773,15 @@
       </c>
       <c r="B37" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C37" s="42">
         <f t="shared" si="2"/>
-        <v>57269932.615358129</v>
+        <v>35828069.844168045</v>
       </c>
       <c r="D37" s="42">
         <f>SUM($C$2:C37)</f>
-        <v>126355325.46773633</v>
+        <v>-764629289.09730303</v>
       </c>
       <c r="M37">
         <v>30</v>
@@ -4831,15 +4817,15 @@
       </c>
       <c r="B38" s="42">
         <f t="shared" si="3"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C38" s="42">
         <f t="shared" si="2"/>
-        <v>-30949185.729372982</v>
+        <v>-52337577.521083787</v>
       </c>
       <c r="D38" s="42">
         <f>SUM($C$2:C38)</f>
-        <v>95406139.738363355</v>
+        <v>-816966866.61838686</v>
       </c>
       <c r="M38">
         <v>31</v>
@@ -4875,15 +4861,15 @@
       </c>
       <c r="B39" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C39" s="42">
         <f t="shared" si="2"/>
-        <v>56984653.195299156</v>
+        <v>35649599.03897915</v>
       </c>
       <c r="D39" s="42">
         <f>SUM($C$2:C39)</f>
-        <v>152390792.9336625</v>
+        <v>-781317267.57940769</v>
       </c>
       <c r="M39">
         <v>32</v>
@@ -4919,15 +4905,15 @@
       </c>
       <c r="B40" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C40" s="42">
         <f t="shared" si="2"/>
-        <v>56842546.8282286</v>
+        <v>35560697.295739815</v>
       </c>
       <c r="D40" s="42">
         <f>SUM($C$2:C40)</f>
-        <v>209233339.7618911</v>
+        <v>-745756570.28366792</v>
       </c>
       <c r="M40">
         <v>33</v>
@@ -4963,15 +4949,15 @@
       </c>
       <c r="B41" s="42">
         <f t="shared" si="3"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C41" s="42">
         <f t="shared" si="2"/>
-        <v>50930921.958092824</v>
+        <v>29702144.369575329</v>
       </c>
       <c r="D41" s="42">
         <f>SUM($C$2:C41)</f>
-        <v>260164261.71998394</v>
+        <v>-716054425.91409254</v>
       </c>
       <c r="M41">
         <v>34</v>
@@ -5007,26 +4993,26 @@
       </c>
       <c r="B42" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C42" s="42">
         <f t="shared" si="2"/>
-        <v>56559396.350250155</v>
+        <v>35383558.356716499</v>
       </c>
       <c r="D42" s="42">
         <f>SUM($C$2:C42)</f>
-        <v>316723658.07023406</v>
+        <v>-680670867.55737603</v>
       </c>
       <c r="M42" t="s">
         <v>17</v>
       </c>
       <c r="N42" s="1">
         <f>SUM(N8:N41)</f>
-        <v>-1726659000</v>
+        <v>-1646659000</v>
       </c>
       <c r="O42" s="1">
         <f t="shared" ref="O42:S42" si="4">SUM(O8:O41)</f>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="P42" s="1">
         <f t="shared" si="4"/>
@@ -5051,15 +5037,15 @@
       </c>
       <c r="B43" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C43" s="42">
         <f t="shared" si="2"/>
-        <v>56418350.474064998</v>
+        <v>35295320.05657506</v>
       </c>
       <c r="D43" s="42">
         <f>SUM($C$2:C43)</f>
-        <v>373142008.54429907</v>
+        <v>-645375547.50080097</v>
       </c>
     </row>
     <row r="44" spans="1:19">
@@ -5068,15 +5054,15 @@
       </c>
       <c r="B44" s="42">
         <f t="shared" si="3"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C44" s="42">
         <f t="shared" si="2"/>
-        <v>50550842.024762243</v>
+        <v>29480487.493600212</v>
       </c>
       <c r="D44" s="42">
         <f>SUM($C$2:C44)</f>
-        <v>423692850.56906128</v>
+        <v>-615895060.00720072</v>
       </c>
     </row>
     <row r="45" spans="1:19">
@@ -5085,15 +5071,15 @@
       </c>
       <c r="B45" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C45" s="42">
         <f t="shared" si="2"/>
-        <v>56137313.050605416</v>
+        <v>35119503.044458747</v>
       </c>
       <c r="D45" s="42">
         <f>SUM($C$2:C45)</f>
-        <v>479830163.6196667</v>
+        <v>-580775556.96274197</v>
       </c>
     </row>
     <row r="46" spans="1:19">
@@ -5102,15 +5088,15 @@
       </c>
       <c r="B46" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C46" s="42">
         <f t="shared" si="2"/>
-        <v>55997319.751227349</v>
+        <v>35031923.236367829</v>
       </c>
       <c r="D46" s="42">
         <f>SUM($C$2:C46)</f>
-        <v>535827483.37089407</v>
+        <v>-545743633.72637415</v>
       </c>
     </row>
     <row r="47" spans="1:19">
@@ -5119,15 +5105,15 @@
       </c>
       <c r="B47" s="42">
         <f t="shared" si="3"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C47" s="42">
         <f t="shared" si="2"/>
-        <v>50173598.497099698</v>
+        <v>29260484.766566515</v>
       </c>
       <c r="D47" s="42">
         <f>SUM($C$2:C47)</f>
-        <v>586001081.86799383</v>
+        <v>-516483148.95980763</v>
       </c>
     </row>
     <row r="48" spans="1:19">
@@ -5136,15 +5122,15 @@
       </c>
       <c r="B48" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C48" s="42">
         <f t="shared" si="2"/>
-        <v>55718379.613288336</v>
+        <v>34857418.286073186</v>
       </c>
       <c r="D48" s="42">
         <f>SUM($C$2:C48)</f>
-        <v>641719461.48128211</v>
+        <v>-481625730.67373443</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -5153,15 +5139,15 @@
       </c>
       <c r="B49" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C49" s="42">
         <f t="shared" si="2"/>
-        <v>55579431.035699092</v>
+        <v>34770492.055933349</v>
       </c>
       <c r="D49" s="42">
         <f>SUM($C$2:C49)</f>
-        <v>697298892.51698124</v>
+        <v>-446855238.61780107</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -5170,15 +5156,15 @@
       </c>
       <c r="B50" s="42">
         <f t="shared" si="3"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C50" s="42">
         <f t="shared" si="2"/>
-        <v>-30035623.499152452</v>
+        <v>-50792669.863008544</v>
       </c>
       <c r="D50" s="42">
         <f>SUM($C$2:C50)</f>
-        <v>667263269.01782882</v>
+        <v>-497647908.48080963</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -5187,15 +5173,15 @@
       </c>
       <c r="B51" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C51" s="42">
         <f t="shared" si="2"/>
-        <v>55302572.531960964</v>
+        <v>34597289.375994779</v>
       </c>
       <c r="D51" s="42">
         <f>SUM($C$2:C51)</f>
-        <v>722565841.54978979</v>
+        <v>-463050619.10481483</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -5204,15 +5190,15 @@
       </c>
       <c r="B52" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C52" s="42">
         <f t="shared" si="2"/>
-        <v>55164660.879761547</v>
+        <v>34511011.846378826</v>
       </c>
       <c r="D52" s="42">
         <f>SUM($C$2:C52)</f>
-        <v>777730502.42955136</v>
+        <v>-428539607.25843602</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -5221,15 +5207,15 @@
       </c>
       <c r="B53" s="42">
         <f t="shared" si="3"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C53" s="42">
         <f t="shared" si="2"/>
-        <v>49427536.14826636</v>
+        <v>28825392.474069122</v>
       </c>
       <c r="D53" s="42">
         <f>SUM($C$2:C53)</f>
-        <v>827158038.57781768</v>
+        <v>-399714214.78436691</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -5238,15 +5224,15 @@
       </c>
       <c r="B54" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C54" s="42">
         <f t="shared" si="2"/>
-        <v>54889868.475705057</v>
+        <v>34339101.718401082</v>
       </c>
       <c r="D54" s="42">
         <f>SUM($C$2:C54)</f>
-        <v>882047907.05352271</v>
+        <v>-365375113.06596583</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -5255,15 +5241,15 @@
       </c>
       <c r="B55" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C55" s="42">
         <f t="shared" si="2"/>
-        <v>54752986.010678366</v>
+        <v>34253468.048280388</v>
       </c>
       <c r="D55" s="42">
         <f>SUM($C$2:C55)</f>
-        <v>936800893.06420112</v>
+        <v>-331121645.01768541</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -5272,15 +5258,15 @@
       </c>
       <c r="B56" s="42">
         <f t="shared" si="3"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C56" s="42">
         <f t="shared" si="2"/>
-        <v>49058675.465567827</v>
+        <v>28610278.495594773</v>
       </c>
       <c r="D56" s="42">
         <f>SUM($C$2:C56)</f>
-        <v>985859568.52976894</v>
+        <v>-302511366.52209061</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -5289,15 +5275,15 @@
       </c>
       <c r="B57" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C57" s="42">
         <f t="shared" si="2"/>
-        <v>54480244.287713014</v>
+        <v>34082840.826393262</v>
       </c>
       <c r="D57" s="42">
         <f>SUM($C$2:C57)</f>
-        <v>1040339812.817482</v>
+        <v>-268428525.69569737</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -5306,15 +5292,15 @@
       </c>
       <c r="B58" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C58" s="42">
         <f t="shared" si="2"/>
-        <v>54344383.32938955</v>
+        <v>33997846.210866101</v>
       </c>
       <c r="D58" s="42">
         <f>SUM($C$2:C58)</f>
-        <v>1094684196.1468716</v>
+        <v>-234430679.48483127</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -5323,15 +5309,15 @@
       </c>
       <c r="B59" s="42">
         <f t="shared" si="3"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C59" s="42">
         <f t="shared" si="2"/>
-        <v>48692567.46313303</v>
+        <v>28396769.838670742</v>
       </c>
       <c r="D59" s="42">
         <f>SUM($C$2:C59)</f>
-        <v>1143376763.6100047</v>
+        <v>-206033909.64616054</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -5340,15 +5326,15 @@
       </c>
       <c r="B60" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C60" s="42">
         <f t="shared" si="2"/>
-        <v>54073676.983988449</v>
+        <v>33828492.321183175</v>
       </c>
       <c r="D60" s="42">
         <f>SUM($C$2:C60)</f>
-        <v>1197450440.5939932</v>
+        <v>-172205417.32497737</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -5357,15 +5343,15 @@
       </c>
       <c r="B61" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C61" s="42">
         <f t="shared" si="2"/>
-        <v>53938829.909215413</v>
+        <v>33744131.991205163</v>
       </c>
       <c r="D61" s="42">
         <f>SUM($C$2:C61)</f>
-        <v>1251389270.5032086</v>
+        <v>-138461285.33377221</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -5374,15 +5360,15 @@
       </c>
       <c r="B62" s="42">
         <f t="shared" si="3"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C62" s="42">
         <f t="shared" si="2"/>
-        <v>-29149027.921812017</v>
+        <v>-49293364.997133963</v>
       </c>
       <c r="D62" s="42">
         <f>SUM($C$2:C62)</f>
-        <v>1222240242.5813966</v>
+        <v>-187754650.33090618</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -5391,15 +5377,15 @@
       </c>
       <c r="B63" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C63" s="42">
         <f t="shared" si="2"/>
-        <v>53670143.752056673</v>
+        <v>33576041.931286655</v>
       </c>
       <c r="D63" s="42">
         <f>SUM($C$2:C63)</f>
-        <v>1275910386.3334532</v>
+        <v>-154178608.39961952</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -5408,15 +5394,15 @@
       </c>
       <c r="B64" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C64" s="42">
         <f t="shared" si="2"/>
-        <v>53536302.994570263</v>
+        <v>33492311.153403159</v>
       </c>
       <c r="D64" s="42">
         <f>SUM($C$2:C64)</f>
-        <v>1329446689.3280234</v>
+        <v>-120686297.24621636</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -5425,15 +5411,15 @@
       </c>
       <c r="B65" s="42">
         <f t="shared" si="3"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C65" s="42">
         <f t="shared" si="2"/>
-        <v>47968527.48313497</v>
+        <v>27974520.659028124</v>
       </c>
       <c r="D65" s="42">
         <f>SUM($C$2:C65)</f>
-        <v>1377415216.8111584</v>
+        <v>-92711776.587188229</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -5442,15 +5428,15 @@
       </c>
       <c r="B66" s="42">
         <f t="shared" si="3"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C66" s="42">
         <f t="shared" ref="C66:C97" si="5">-PV($K$1,A66,,B66)</f>
-        <v>53269621.949684657</v>
+        <v>33325475.491722722</v>
       </c>
       <c r="D66" s="42">
         <f>SUM($C$2:C66)</f>
-        <v>1430684838.760843</v>
+        <v>-59386301.095465511</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -5459,15 +5445,15 @@
       </c>
       <c r="B67" s="42">
         <f t="shared" ref="B67:B98" si="6">IF(A67=0,$N$42,0)+IF(A67=0,0,$O$42)+IF(MOD(A67,2)=0,$P$42,0)+IF(MOD(A67,3)=0,$Q$42,0)+IF(MOD(A67,6)=0,$R$42,0)+IF(MOD(A67,12)=0,$S$42,0)</f>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C67" s="42">
         <f t="shared" si="5"/>
-        <v>53136779.999685444</v>
+        <v>33242369.567803212</v>
       </c>
       <c r="D67" s="42">
         <f>SUM($C$2:C67)</f>
-        <v>1483821618.7605286</v>
+        <v>-26143931.5276623</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -5476,15 +5462,15 @@
       </c>
       <c r="B68" s="42">
         <f t="shared" si="6"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C68" s="42">
         <f t="shared" si="5"/>
-        <v>47610554.879718162</v>
+        <v>27765756.443925411</v>
       </c>
       <c r="D68" s="42">
         <f>SUM($C$2:C68)</f>
-        <v>1531432173.6402466</v>
+        <v>1621824.9162631109</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -5493,15 +5479,15 @@
       </c>
       <c r="B69" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C69" s="42">
         <f t="shared" si="5"/>
-        <v>52872089.103610501</v>
+        <v>33076778.94321873</v>
       </c>
       <c r="D69" s="42">
         <f>SUM($C$2:C69)</f>
-        <v>1584304262.7438571</v>
+        <v>34698603.859481841</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -5510,15 +5496,15 @@
       </c>
       <c r="B70" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C70" s="42">
         <f t="shared" si="5"/>
-        <v>52740238.507342145</v>
+        <v>32994293.210193247</v>
       </c>
       <c r="D70" s="42">
         <f>SUM($C$2:C70)</f>
-        <v>1637044501.2511992</v>
+        <v>67692897.069675088</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -5527,15 +5513,15 @@
       </c>
       <c r="B71" s="42">
         <f t="shared" si="6"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C71" s="42">
         <f t="shared" si="5"/>
-        <v>47255253.702578567</v>
+        <v>27558550.164275423</v>
       </c>
       <c r="D71" s="42">
         <f>SUM($C$2:C71)</f>
-        <v>1684299754.9537778</v>
+        <v>95251447.233950511</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -5544,15 +5530,15 @@
       </c>
       <c r="B72" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C72" s="42">
         <f t="shared" si="5"/>
-        <v>52477522.908282571</v>
+        <v>32829938.331421573</v>
       </c>
       <c r="D72" s="42">
         <f>SUM($C$2:C72)</f>
-        <v>1736777277.8620603</v>
+        <v>128081385.56537208</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -5561,15 +5547,15 @@
       </c>
       <c r="B73" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C73" s="42">
         <f t="shared" si="5"/>
-        <v>52346656.267613538</v>
+        <v>32748068.161019031</v>
       </c>
       <c r="D73" s="42">
         <f>SUM($C$2:C73)</f>
-        <v>1789123934.129674</v>
+        <v>160829453.72639111</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -5578,15 +5564,15 @@
       </c>
       <c r="B74" s="42">
         <f t="shared" si="6"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C74" s="42">
         <f t="shared" si="5"/>
-        <v>-28288602.992062155</v>
+        <v>-47838316.814101562</v>
       </c>
       <c r="D74" s="42">
         <f>SUM($C$2:C74)</f>
-        <v>1760835331.1376119</v>
+        <v>112991136.91228954</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -5595,15 +5581,15 @@
       </c>
       <c r="B75" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C75" s="42">
         <f t="shared" si="5"/>
-        <v>52085901.224607848</v>
+        <v>32584939.806114666</v>
       </c>
       <c r="D75" s="42">
         <f>SUM($C$2:C75)</f>
-        <v>1812921232.3622198</v>
+        <v>145576076.7184042</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -5612,15 +5598,15 @@
       </c>
       <c r="B76" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C76" s="42">
         <f t="shared" si="5"/>
-        <v>51956011.196616307</v>
+        <v>32503680.60460316</v>
       </c>
       <c r="D76" s="42">
         <f>SUM($C$2:C76)</f>
-        <v>1864877243.5588362</v>
+        <v>178079757.32300738</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -5629,15 +5615,15 @@
       </c>
       <c r="B77" s="42">
         <f t="shared" si="6"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C77" s="42">
         <f t="shared" si="5"/>
-        <v>46552586.032168217</v>
+        <v>27148764.992753606</v>
       </c>
       <c r="D77" s="42">
         <f>SUM($C$2:C77)</f>
-        <v>1911429829.5910044</v>
+        <v>205228522.31576097</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -5646,15 +5632,15 @@
       </c>
       <c r="B78" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C78" s="42">
         <f t="shared" si="5"/>
-        <v>51697202.078709774</v>
+        <v>32341769.620440833</v>
       </c>
       <c r="D78" s="42">
         <f>SUM($C$2:C78)</f>
-        <v>1963127031.6697142</v>
+        <v>237570291.93620181</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -5663,15 +5649,15 @@
       </c>
       <c r="B79" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C79" s="42">
         <f t="shared" si="5"/>
-        <v>51568281.375271589</v>
+        <v>32261116.828369904</v>
       </c>
       <c r="D79" s="42">
         <f>SUM($C$2:C79)</f>
-        <v>2014695313.0449858</v>
+        <v>269831408.76457173</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -5680,15 +5666,15 @@
       </c>
       <c r="B80" s="42">
         <f t="shared" si="6"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C80" s="42">
         <f t="shared" si="5"/>
-        <v>46205180.112243354</v>
+        <v>26946163.107852645</v>
       </c>
       <c r="D80" s="42">
         <f>SUM($C$2:C80)</f>
-        <v>2060900493.1572292</v>
+        <v>296777571.87242436</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -5697,15 +5683,15 @@
       </c>
       <c r="B81" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C81" s="42">
         <f t="shared" si="5"/>
-        <v>51311403.660695247</v>
+        <v>32100414.13013095</v>
       </c>
       <c r="D81" s="42">
         <f>SUM($C$2:C81)</f>
-        <v>2112211896.8179245</v>
+        <v>328877986.00255531</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -5714,15 +5700,15 @@
       </c>
       <c r="B82" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C82" s="42">
         <f t="shared" si="5"/>
-        <v>51183445.048075058</v>
+        <v>32020363.222075753</v>
       </c>
       <c r="D82" s="42">
         <f>SUM($C$2:C82)</f>
-        <v>2163395341.8659997</v>
+        <v>360898349.22463107</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -5731,15 +5717,15 @@
       </c>
       <c r="B83" s="42">
         <f t="shared" si="6"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C83" s="42">
         <f t="shared" si="5"/>
-        <v>45860366.763075262</v>
+        <v>26745073.171056002</v>
       </c>
       <c r="D83" s="42">
         <f>SUM($C$2:C83)</f>
-        <v>2209255708.6290751</v>
+        <v>387643422.3956871</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -5748,15 +5734,15 @@
       </c>
       <c r="B84" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C84" s="42">
         <f t="shared" si="5"/>
-        <v>50928484.323430881</v>
+        <v>31860859.792738356</v>
       </c>
       <c r="D84" s="42">
         <f>SUM($C$2:C84)</f>
-        <v>2260184192.9525061</v>
+        <v>419504282.18842548</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -5765,15 +5751,15 @@
       </c>
       <c r="B85" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C85" s="42">
         <f t="shared" si="5"/>
-        <v>50801480.621876195</v>
+        <v>31781406.277045749</v>
       </c>
       <c r="D85" s="42">
         <f>SUM($C$2:C85)</f>
-        <v>2310985673.5743823</v>
+        <v>451285688.46547121</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -5782,15 +5768,15 @@
       </c>
       <c r="B86" s="42">
         <f t="shared" si="6"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C86" s="42">
         <f t="shared" si="5"/>
-        <v>-27453576.201204639</v>
+        <v>-46426218.93919012</v>
       </c>
       <c r="D86" s="42">
         <f>SUM($C$2:C86)</f>
-        <v>2283532097.3731775</v>
+        <v>404859469.52628112</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -5799,15 +5785,15 @@
       </c>
       <c r="B87" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C87" s="42">
         <f t="shared" si="5"/>
-        <v>50548422.581328422</v>
+        <v>31623093.166879062</v>
       </c>
       <c r="D87" s="42">
         <f>SUM($C$2:C87)</f>
-        <v>2334080519.9545059</v>
+        <v>436482562.69316018</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -5816,15 +5802,15 @@
       </c>
       <c r="B88" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C88" s="42">
         <f t="shared" si="5"/>
-        <v>50422366.664666772</v>
+        <v>31544232.585415535</v>
       </c>
       <c r="D88" s="42">
         <f>SUM($C$2:C88)</f>
-        <v>2384502886.6191726</v>
+        <v>468026795.27857572</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -5833,15 +5819,15 @@
       </c>
       <c r="B89" s="42">
         <f t="shared" si="6"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C89" s="42">
         <f t="shared" si="5"/>
-        <v>45178440.531541422</v>
+        <v>26347384.093385577</v>
       </c>
       <c r="D89" s="42">
         <f>SUM($C$2:C89)</f>
-        <v>2429681327.1507139</v>
+        <v>494374179.3719613</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -5850,15 +5836,15 @@
       </c>
       <c r="B90" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C90" s="42">
         <f t="shared" si="5"/>
-        <v>50171197.109139144</v>
+        <v>31387100.911477447</v>
       </c>
       <c r="D90" s="42">
         <f>SUM($C$2:C90)</f>
-        <v>2479852524.2598529</v>
+        <v>525761280.28343874</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -5867,15 +5853,15 @@
       </c>
       <c r="B91" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C91" s="42">
         <f t="shared" si="5"/>
-        <v>50046081.904378191</v>
+        <v>31308828.839378998</v>
       </c>
       <c r="D91" s="42">
         <f>SUM($C$2:C91)</f>
-        <v>2529898606.1642313</v>
+        <v>557070109.12281775</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -5884,15 +5870,15 @@
       </c>
       <c r="B92" s="42">
         <f t="shared" si="6"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C92" s="42">
         <f t="shared" si="5"/>
-        <v>44841289.386322856</v>
+        <v>26150762.638193987</v>
       </c>
       <c r="D92" s="42">
         <f>SUM($C$2:C92)</f>
-        <v>2574739895.5505543</v>
+        <v>583220871.76101172</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -5901,15 +5887,15 @@
       </c>
       <c r="B93" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C93" s="42">
         <f t="shared" si="5"/>
-        <v>49796786.740757287</v>
+        <v>31152869.785017755</v>
       </c>
       <c r="D93" s="42">
         <f>SUM($C$2:C93)</f>
-        <v>2624536682.2913117</v>
+        <v>614373741.54602945</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -5918,15 +5904,15 @@
       </c>
       <c r="B94" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C94" s="42">
         <f t="shared" si="5"/>
-        <v>49672605.227688067</v>
+        <v>31075181.830441657</v>
       </c>
       <c r="D94" s="42">
         <f>SUM($C$2:C94)</f>
-        <v>2674209287.5189996</v>
+        <v>645448923.37647116</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -5935,15 +5921,15 @@
       </c>
       <c r="B95" s="42">
         <f t="shared" si="6"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C95" s="42">
         <f t="shared" si="5"/>
-        <v>44506654.284008496</v>
+        <v>25955608.501219064</v>
       </c>
       <c r="D95" s="42">
         <f>SUM($C$2:C95)</f>
-        <v>2718715941.8030081</v>
+        <v>671404531.8776902</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -5952,15 +5938,15 @@
       </c>
       <c r="B96" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C96" s="42">
         <f t="shared" si="5"/>
-        <v>49425170.468032487</v>
+        <v>30920386.644801121</v>
       </c>
       <c r="D96" s="42">
         <f>SUM($C$2:C96)</f>
-        <v>2768141112.2710404</v>
+        <v>702324918.52249134</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -5969,15 +5955,15 @@
       </c>
       <c r="B97" s="42">
         <f t="shared" si="6"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C97" s="42">
         <f t="shared" si="5"/>
-        <v>49301915.678835399</v>
+        <v>30843278.448679429</v>
       </c>
       <c r="D97" s="42">
         <f>SUM($C$2:C97)</f>
-        <v>2817443027.9498758</v>
+        <v>733168196.97117078</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -5986,15 +5972,15 @@
       </c>
       <c r="B98" s="42">
         <f t="shared" si="6"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C98" s="42">
         <f t="shared" ref="C98:C129" si="7">-PV($K$1,A98,,B98)</f>
-        <v>-26643197.84355697</v>
+        <v>-45055803.559423275</v>
       </c>
       <c r="D98" s="42">
         <f>SUM($C$2:C98)</f>
-        <v>2790799830.106319</v>
+        <v>688112393.41174746</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -6003,15 +5989,15 @@
       </c>
       <c r="B99" s="42">
         <f t="shared" ref="B99:B130" si="8">IF(A99=0,$N$42,0)+IF(A99=0,0,$O$42)+IF(MOD(A99,2)=0,$P$42,0)+IF(MOD(A99,3)=0,$Q$42,0)+IF(MOD(A99,6)=0,$R$42,0)+IF(MOD(A99,12)=0,$S$42,0)</f>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C99" s="42">
         <f t="shared" si="7"/>
-        <v>49056327.439590938</v>
+        <v>30689638.446208093</v>
       </c>
       <c r="D99" s="42">
         <f>SUM($C$2:C99)</f>
-        <v>2839856157.5459099</v>
+        <v>718802031.85795557</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -6020,15 +6006,15 @@
       </c>
       <c r="B100" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C100" s="42">
         <f t="shared" si="7"/>
-        <v>48933992.458444841</v>
+        <v>30613105.682003092</v>
       </c>
       <c r="D100" s="42">
         <f>SUM($C$2:C100)</f>
-        <v>2888790150.004355</v>
+        <v>749415137.53995872</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -6037,15 +6023,15 @@
       </c>
       <c r="B101" s="42">
         <f t="shared" si="8"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C101" s="42">
         <f t="shared" si="7"/>
-        <v>43844857.242766581</v>
+        <v>25569658.463273562</v>
       </c>
       <c r="D101" s="42">
         <f>SUM($C$2:C101)</f>
-        <v>2932635007.2471213</v>
+        <v>774984796.00323224</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -6054,15 +6040,15 @@
       </c>
       <c r="B102" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C102" s="42">
         <f t="shared" si="7"/>
-        <v>48690236.959665507</v>
+        <v>30460612.241966743</v>
       </c>
       <c r="D102" s="42">
         <f>SUM($C$2:C102)</f>
-        <v>2981325244.2067866</v>
+        <v>805445408.24519897</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -6071,15 +6057,15 @@
       </c>
       <c r="B103" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C103" s="42">
         <f t="shared" si="7"/>
-        <v>48568814.922359608</v>
+        <v>30384650.615428172</v>
       </c>
       <c r="D103" s="42">
         <f>SUM($C$2:C103)</f>
-        <v>3029894059.1291461</v>
+        <v>835830058.86062717</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -6088,15 +6074,15 @@
       </c>
       <c r="B104" s="42">
         <f t="shared" si="8"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C104" s="42">
         <f t="shared" si="7"/>
-        <v>43517658.170434229</v>
+        <v>25378840.906662211</v>
       </c>
       <c r="D104" s="42">
         <f>SUM($C$2:C104)</f>
-        <v>3073411717.2995801</v>
+        <v>861208899.7672894</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -6105,15 +6091,15 @@
       </c>
       <c r="B105" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C105" s="42">
         <f t="shared" si="7"/>
-        <v>48326878.486934409</v>
+        <v>30233295.181426164</v>
       </c>
       <c r="D105" s="42">
         <f>SUM($C$2:C105)</f>
-        <v>3121738595.7865143</v>
+        <v>891442194.94871557</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -6122,15 +6108,15 @@
       </c>
       <c r="B106" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C106" s="42">
         <f t="shared" si="7"/>
-        <v>48206362.580483198</v>
+        <v>30157900.430350289</v>
       </c>
       <c r="D106" s="42">
         <f>SUM($C$2:C106)</f>
-        <v>3169944958.3669977</v>
+        <v>921600095.37906587</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -6139,15 +6125,15 @@
       </c>
       <c r="B107" s="42">
         <f t="shared" si="8"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C107" s="42">
         <f t="shared" si="7"/>
-        <v>43192900.872112952</v>
+        <v>25189447.355770893</v>
       </c>
       <c r="D107" s="42">
         <f>SUM($C$2:C107)</f>
-        <v>3213137859.2391105</v>
+        <v>946789542.73483682</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -6156,15 +6142,15 @@
       </c>
       <c r="B108" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C108" s="42">
         <f t="shared" si="7"/>
-        <v>47966231.633368656</v>
+        <v>30007674.509835433</v>
       </c>
       <c r="D108" s="42">
         <f>SUM($C$2:C108)</f>
-        <v>3261104090.872479</v>
+        <v>976797217.2446723</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -6173,15 +6159,15 @@
       </c>
       <c r="B109" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C109" s="42">
         <f t="shared" si="7"/>
-        <v>47846615.095629588</v>
+        <v>29932842.403825868</v>
       </c>
       <c r="D109" s="42">
         <f>SUM($C$2:C109)</f>
-        <v>3308950705.9681087</v>
+        <v>1006730059.6484982</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -6190,15 +6176,15 @@
       </c>
       <c r="B110" s="42">
         <f t="shared" si="8"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C110" s="42">
         <f t="shared" si="7"/>
-        <v>-25856740.343349911</v>
+        <v>-43725840.285298757</v>
       </c>
       <c r="D110" s="42">
         <f>SUM($C$2:C110)</f>
-        <v>3283093965.6247587</v>
+        <v>963004219.36319947</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -6207,15 +6193,15 @@
       </c>
       <c r="B111" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C111" s="42">
         <f t="shared" si="7"/>
-        <v>47608276.163088121</v>
+        <v>29783737.567627929</v>
       </c>
       <c r="D111" s="42">
         <f>SUM($C$2:C111)</f>
-        <v>3330702241.787847</v>
+        <v>992787956.93082738</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -6224,15 +6210,15 @@
       </c>
       <c r="B112" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C112" s="42">
         <f t="shared" si="7"/>
-        <v>47489552.282382183</v>
+        <v>29709463.907858294</v>
       </c>
       <c r="D112" s="42">
         <f>SUM($C$2:C112)</f>
-        <v>3378191794.0702291</v>
+        <v>1022497420.8386856</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -6241,15 +6227,15 @@
       </c>
       <c r="B113" s="42">
         <f t="shared" si="8"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C113" s="42">
         <f t="shared" si="7"/>
-        <v>42550638.845014438</v>
+        <v>24814889.842995595</v>
       </c>
       <c r="D113" s="42">
         <f>SUM($C$2:C113)</f>
-        <v>3420742432.9152436</v>
+        <v>1047312310.6816813</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -6258,15 +6244,15 @@
       </c>
       <c r="B114" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C114" s="42">
         <f t="shared" si="7"/>
-        <v>47252991.991226092</v>
+        <v>29561471.789711043</v>
       </c>
       <c r="D114" s="42">
         <f>SUM($C$2:C114)</f>
-        <v>3467995424.9064698</v>
+        <v>1076873782.4713924</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -6275,15 +6261,15 @@
       </c>
       <c r="B115" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C115" s="42">
         <f t="shared" si="7"/>
-        <v>47135154.105961204</v>
+        <v>29487752.408689331</v>
       </c>
       <c r="D115" s="42">
         <f>SUM($C$2:C115)</f>
-        <v>3515130579.0124311</v>
+        <v>1106361534.8800817</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -6292,15 +6278,15 @@
       </c>
       <c r="B116" s="42">
         <f t="shared" si="8"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C116" s="42">
         <f t="shared" si="7"/>
-        <v>42233098.078941233</v>
+        <v>24629704.864704952</v>
       </c>
       <c r="D116" s="42">
         <f>SUM($C$2:C116)</f>
-        <v>3557363677.0913725</v>
+        <v>1130991239.7447865</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -6309,15 +6295,15 @@
       </c>
       <c r="B117" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C117" s="42">
         <f t="shared" si="7"/>
-        <v>46900359.182802305</v>
+        <v>29340864.704761121</v>
       </c>
       <c r="D117" s="42">
         <f>SUM($C$2:C117)</f>
-        <v>3604264036.2741747</v>
+        <v>1160332104.4495475</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -6326,15 +6312,15 @@
       </c>
       <c r="B118" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C118" s="42">
         <f t="shared" si="7"/>
-        <v>46783400.681099556</v>
+        <v>29267695.46609588</v>
       </c>
       <c r="D118" s="42">
         <f>SUM($C$2:C118)</f>
-        <v>3651047436.9552741</v>
+        <v>1189599799.9156435</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -6343,15 +6329,15 @@
       </c>
       <c r="B119" s="42">
         <f t="shared" si="8"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C119" s="42">
         <f t="shared" si="7"/>
-        <v>41917927.010265201</v>
+        <v>24445901.858141836</v>
       </c>
       <c r="D119" s="42">
         <f>SUM($C$2:C119)</f>
-        <v>3692965363.9655395</v>
+        <v>1214045701.7737854</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -6360,15 +6346,15 @@
       </c>
       <c r="B120" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C120" s="42">
         <f t="shared" si="7"/>
-        <v>46550357.951604351</v>
+        <v>29121903.934523679</v>
       </c>
       <c r="D120" s="42">
         <f>SUM($C$2:C120)</f>
-        <v>3739515721.9171438</v>
+        <v>1243167605.7083089</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -6377,15 +6363,15 @@
       </c>
       <c r="B121" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C121" s="42">
         <f t="shared" si="7"/>
-        <v>46434272.270927034</v>
+        <v>29049280.732691951</v>
       </c>
       <c r="D121" s="42">
         <f>SUM($C$2:C121)</f>
-        <v>3785949994.1880708</v>
+        <v>1272216886.4410009</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -6394,15 +6380,15 @@
       </c>
       <c r="B122" s="42">
         <f t="shared" si="8"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C122" s="42">
         <f t="shared" si="7"/>
-        <v>-25093497.601493698</v>
+        <v>-42435135.046117224</v>
       </c>
       <c r="D122" s="42">
         <f>SUM($C$2:C122)</f>
-        <v>3760856496.5865769</v>
+        <v>1229781751.3948836</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -6411,15 +6397,15 @@
       </c>
       <c r="B123" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C123" s="42">
         <f t="shared" si="7"/>
-        <v>46202968.659077525</v>
+        <v>28904577.1931189</v>
       </c>
       <c r="D123" s="42">
         <f>SUM($C$2:C123)</f>
-        <v>3807059465.2456546</v>
+        <v>1258686328.5880024</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -6428,15 +6414,15 @@
       </c>
       <c r="B124" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C124" s="42">
         <f t="shared" si="7"/>
-        <v>46087749.285862871</v>
+        <v>28832495.953235809</v>
       </c>
       <c r="D124" s="42">
         <f>SUM($C$2:C124)</f>
-        <v>3853147214.5315175</v>
+        <v>1287518824.5412383</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -6445,15 +6431,15 @@
       </c>
       <c r="B125" s="42">
         <f t="shared" si="8"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C125" s="42">
         <f t="shared" si="7"/>
-        <v>41294623.360133126</v>
+        <v>24082400.58444529</v>
       </c>
       <c r="D125" s="42">
         <f>SUM($C$2:C125)</f>
-        <v>3894441837.8916507</v>
+        <v>1311601225.1256835</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -6462,15 +6448,15 @@
       </c>
       <c r="B126" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C126" s="42">
         <f t="shared" si="7"/>
-        <v>45858171.813222922</v>
+        <v>28688872.286352262</v>
       </c>
       <c r="D126" s="42">
         <f>SUM($C$2:C126)</f>
-        <v>3940300009.7048736</v>
+        <v>1340290097.4120357</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -6479,15 +6465,15 @@
       </c>
       <c r="B127" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C127" s="42">
         <f t="shared" si="7"/>
-        <v>45743812.282516629</v>
+        <v>28617328.963942401</v>
       </c>
       <c r="D127" s="42">
         <f>SUM($C$2:C127)</f>
-        <v>3986043821.98739</v>
+        <v>1368907426.375978</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -6496,15 +6482,15 @@
       </c>
       <c r="B128" s="42">
         <f t="shared" si="8"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C128" s="42">
         <f t="shared" si="7"/>
-        <v>40986455.805134907</v>
+        <v>23902681.921270341</v>
       </c>
       <c r="D128" s="42">
         <f>SUM($C$2:C128)</f>
-        <v>4027030277.7925248</v>
+        <v>1392810108.2972484</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -6513,15 +6499,15 @@
       </c>
       <c r="B129" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C129" s="42">
         <f t="shared" si="7"/>
-        <v>45515948.067503713</v>
+        <v>28474777.111030322</v>
       </c>
       <c r="D129" s="42">
         <f>SUM($C$2:C129)</f>
-        <v>4072546225.8600287</v>
+        <v>1421284885.4082787</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -6530,15 +6516,15 @@
       </c>
       <c r="B130" s="42">
         <f t="shared" si="8"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C130" s="42">
         <f t="shared" ref="C130:C168" si="9">-PV($K$1,A130,,B130)</f>
-        <v>45402441.962597206</v>
+        <v>28403767.691800814</v>
       </c>
       <c r="D130" s="42">
         <f>SUM($C$2:C130)</f>
-        <v>4117948667.8226261</v>
+        <v>1449688653.1000795</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -6547,15 +6533,15 @@
       </c>
       <c r="B131" s="42">
         <f t="shared" ref="B131:B162" si="10">IF(A131=0,$N$42,0)+IF(A131=0,0,$O$42)+IF(MOD(A131,2)=0,$P$42,0)+IF(MOD(A131,3)=0,$Q$42,0)+IF(MOD(A131,6)=0,$R$42,0)+IF(MOD(A131,12)=0,$S$42,0)</f>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C131" s="42">
         <f t="shared" si="9"/>
-        <v>40680587.9984871</v>
+        <v>23724304.436595432</v>
       </c>
       <c r="D131" s="42">
         <f>SUM($C$2:C131)</f>
-        <v>4158629255.8211131</v>
+        <v>1473412957.536675</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -6564,15 +6550,15 @@
       </c>
       <c r="B132" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C132" s="42">
         <f t="shared" si="9"/>
-        <v>45176278.219759539</v>
+        <v>28262279.654281568</v>
       </c>
       <c r="D132" s="42">
         <f>SUM($C$2:C132)</f>
-        <v>4203805534.0408726</v>
+        <v>1501675237.1909566</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -6581,15 +6567,15 @@
       </c>
       <c r="B133" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C133" s="42">
         <f t="shared" si="9"/>
-        <v>45063619.171829969</v>
+        <v>28191800.153896831</v>
       </c>
       <c r="D133" s="42">
         <f>SUM($C$2:C133)</f>
-        <v>4248869153.2127028</v>
+        <v>1529867037.3448534</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -6598,15 +6584,15 @@
       </c>
       <c r="B134" s="42">
         <f t="shared" si="10"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C134" s="42">
         <f t="shared" si="9"/>
-        <v>-24352784.361626539</v>
+        <v>-41182529.017918952</v>
       </c>
       <c r="D134" s="42">
         <f>SUM($C$2:C134)</f>
-        <v>4224516368.8510761</v>
+        <v>1488684508.3269343</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -6615,15 +6601,15 @@
       </c>
       <c r="B135" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C135" s="42">
         <f t="shared" si="9"/>
-        <v>44839143.211129256</v>
+        <v>28051367.992882464</v>
       </c>
       <c r="D135" s="42">
         <f>SUM($C$2:C135)</f>
-        <v>4269355512.0622053</v>
+        <v>1516735876.3198168</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -6632,15 +6618,15 @@
       </c>
       <c r="B136" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C136" s="42">
         <f t="shared" si="9"/>
-        <v>44727324.898882061</v>
+        <v>27981414.456740618</v>
       </c>
       <c r="D136" s="42">
         <f>SUM($C$2:C136)</f>
-        <v>4314082836.9610872</v>
+        <v>1544717290.7765574</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -6649,15 +6635,15 @@
       </c>
       <c r="B137" s="42">
         <f t="shared" si="10"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C137" s="42">
         <f t="shared" si="9"/>
-        <v>40075683.109398328</v>
+        <v>23371533.042424317</v>
       </c>
       <c r="D137" s="42">
         <f>SUM($C$2:C137)</f>
-        <v>4354158520.0704851</v>
+        <v>1568088823.8189816</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -6666,15 +6652,15 @@
       </c>
       <c r="B138" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C138" s="42">
         <f t="shared" si="9"/>
-        <v>44504524.124981366</v>
+        <v>27842030.292588342</v>
       </c>
       <c r="D138" s="42">
         <f>SUM($C$2:C138)</f>
-        <v>4398663044.195466</v>
+        <v>1595930854.1115699</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -6683,15 +6669,15 @@
       </c>
       <c r="B139" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C139" s="42">
         <f t="shared" si="9"/>
-        <v>44393540.274295628</v>
+        <v>27772598.795599345</v>
       </c>
       <c r="D139" s="42">
         <f>SUM($C$2:C139)</f>
-        <v>4443056584.4697618</v>
+        <v>1623703452.9071693</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -6700,15 +6686,15 @@
       </c>
       <c r="B140" s="42">
         <f t="shared" si="10"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C140" s="42">
         <f t="shared" si="9"/>
-        <v>39776612.085768886</v>
+        <v>23197119.338939678</v>
       </c>
       <c r="D140" s="42">
         <f>SUM($C$2:C140)</f>
-        <v>4482833196.5555305</v>
+        <v>1646900572.246109</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -6717,15 +6703,15 @@
       </c>
       <c r="B141" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C141" s="42">
         <f t="shared" si="9"/>
-        <v>44172402.185852721</v>
+        <v>27634254.807469461</v>
       </c>
       <c r="D141" s="42">
         <f>SUM($C$2:C141)</f>
-        <v>4527005598.7413836</v>
+        <v>1674534827.0535784</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -6734,15 +6720,15 @@
       </c>
       <c r="B142" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C142" s="42">
         <f t="shared" si="9"/>
-        <v>44062246.569429137</v>
+        <v>27565341.453834869</v>
       </c>
       <c r="D142" s="42">
         <f>SUM($C$2:C142)</f>
-        <v>4571067845.310813</v>
+        <v>1702100168.5074131</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -6751,15 +6737,15 @@
       </c>
       <c r="B143" s="42">
         <f t="shared" si="10"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C143" s="42">
         <f t="shared" si="9"/>
-        <v>39479772.926208511</v>
+        <v>23024007.22486759</v>
       </c>
       <c r="D143" s="42">
         <f>SUM($C$2:C143)</f>
-        <v>4610547618.2370214</v>
+        <v>1725124175.7322807</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -6768,15 +6754,15 @@
       </c>
       <c r="B144" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C144" s="42">
         <f t="shared" si="9"/>
-        <v>43842758.758394934</v>
+        <v>27428029.879251871</v>
       </c>
       <c r="D144" s="42">
         <f>SUM($C$2:C144)</f>
-        <v>4654390376.9954166</v>
+        <v>1752552205.6115327</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -6785,15 +6771,15 @@
       </c>
       <c r="B145" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C145" s="42">
         <f t="shared" si="9"/>
-        <v>43733425.195406422</v>
+        <v>27359630.802246261</v>
       </c>
       <c r="D145" s="42">
         <f>SUM($C$2:C145)</f>
-        <v>4698123802.1908226</v>
+        <v>1779911836.413779</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -6802,15 +6788,15 @@
       </c>
       <c r="B146" s="42">
         <f t="shared" si="10"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C146" s="42">
         <f t="shared" si="9"/>
-        <v>-23633935.594876193</v>
+        <v>-39966897.583065882</v>
       </c>
       <c r="D146" s="42">
         <f>SUM($C$2:C146)</f>
-        <v>4674489866.5959463</v>
+        <v>1739944938.830713</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -6819,15 +6805,15 @@
       </c>
       <c r="B147" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C147" s="42">
         <f t="shared" si="9"/>
-        <v>43515575.346328862</v>
+        <v>27223343.936663337</v>
       </c>
       <c r="D147" s="42">
         <f>SUM($C$2:C147)</f>
-        <v>4718005441.942275</v>
+        <v>1767168282.7673764</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -6836,15 +6822,15 @@
       </c>
       <c r="B148" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C148" s="42">
         <f t="shared" si="9"/>
-        <v>43407057.702073671</v>
+        <v>27155455.298417289</v>
       </c>
       <c r="D148" s="42">
         <f>SUM($C$2:C148)</f>
-        <v>4761412499.6443491</v>
+        <v>1794323738.0657938</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -6853,15 +6839,15 @@
       </c>
       <c r="B149" s="42">
         <f t="shared" si="10"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C149" s="42">
         <f t="shared" si="9"/>
-        <v>38892723.701058023</v>
+        <v>22681648.984193794</v>
       </c>
       <c r="D149" s="42">
         <f>SUM($C$2:C149)</f>
-        <v>4800305223.3454075</v>
+        <v>1817005387.0499876</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -6870,15 +6856,15 @@
       </c>
       <c r="B150" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C150" s="42">
         <f t="shared" si="9"/>
-        <v>43190833.591406696</v>
+        <v>27020185.494784031</v>
       </c>
       <c r="D150" s="42">
         <f>SUM($C$2:C150)</f>
-        <v>4843496056.9368143</v>
+        <v>1844025572.5447717</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -6887,15 +6873,15 @@
       </c>
       <c r="B151" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C151" s="42">
         <f t="shared" si="9"/>
-        <v>43083125.776964299</v>
+        <v>26952803.486068863</v>
       </c>
       <c r="D151" s="42">
         <f>SUM($C$2:C151)</f>
-        <v>4886579182.7137785</v>
+        <v>1870978376.0308406</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -6904,15 +6890,15 @@
       </c>
       <c r="B152" s="42">
         <f t="shared" si="10"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C152" s="42">
         <f t="shared" si="9"/>
-        <v>38602480.696160018</v>
+        <v>22512383.64788527</v>
       </c>
       <c r="D152" s="42">
         <f>SUM($C$2:C152)</f>
-        <v>4925181663.4099388</v>
+        <v>1893490759.678726</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -6921,15 +6907,15 @@
       </c>
       <c r="B153" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C153" s="42">
         <f t="shared" si="9"/>
-        <v>42868515.272381939</v>
+        <v>26818543.154402144</v>
       </c>
       <c r="D153" s="42">
         <f>SUM($C$2:C153)</f>
-        <v>4968050178.6823206</v>
+        <v>1920309302.8331282</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -6938,15 +6924,15 @@
       </c>
       <c r="B154" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C154" s="42">
         <f t="shared" si="9"/>
-        <v>42761611.244271263</v>
+        <v>26751663.994416103</v>
       </c>
       <c r="D154" s="42">
         <f>SUM($C$2:C154)</f>
-        <v>5010811789.9265919</v>
+        <v>1947060966.8275442</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -6955,15 +6941,15 @@
       </c>
       <c r="B155" s="42">
         <f t="shared" si="10"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C155" s="42">
         <f t="shared" si="9"/>
-        <v>38314403.674867049</v>
+        <v>22344381.480497811</v>
       </c>
       <c r="D155" s="42">
         <f>SUM($C$2:C155)</f>
-        <v>5049126193.6014585</v>
+        <v>1969405348.308042</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -6972,15 +6958,15 @@
       </c>
       <c r="B156" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C156" s="42">
         <f t="shared" si="9"/>
-        <v>42548602.303986929</v>
+        <v>26618405.601374224</v>
       </c>
       <c r="D156" s="42">
         <f>SUM($C$2:C156)</f>
-        <v>5091674795.9054451</v>
+        <v>1996023753.9094162</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -6989,15 +6975,15 @@
       </c>
       <c r="B157" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C157" s="42">
         <f t="shared" si="9"/>
-        <v>42442496.063827366</v>
+        <v>26552025.5375304</v>
       </c>
       <c r="D157" s="42">
         <f>SUM($C$2:C157)</f>
-        <v>5134117291.9692726</v>
+        <v>2022575779.4469466</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -7006,15 +6992,15 @@
       </c>
       <c r="B158" s="42">
         <f t="shared" si="10"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C158" s="42">
         <f t="shared" si="9"/>
-        <v>-22936305.902782161</v>
+        <v>-38787149.320534743</v>
       </c>
       <c r="D158" s="42">
         <f>SUM($C$2:C158)</f>
-        <v>5111180986.0664902</v>
+        <v>1983788630.1264119</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -7023,15 +7009,15 @@
       </c>
       <c r="B159" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C159" s="42">
         <f t="shared" si="9"/>
-        <v>42231076.735918172</v>
+        <v>26419761.605990406</v>
       </c>
       <c r="D159" s="42">
         <f>SUM($C$2:C159)</f>
-        <v>5153412062.8024082</v>
+        <v>2010208391.7324023</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -7040,15 +7026,15 @@
       </c>
       <c r="B160" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C160" s="42">
         <f t="shared" si="9"/>
-        <v>42125762.330092952</v>
+        <v>26353876.91370615</v>
       </c>
       <c r="D160" s="42">
         <f>SUM($C$2:C160)</f>
-        <v>5195537825.1325016</v>
+        <v>2036562268.6461084</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -7057,15 +7043,15 @@
       </c>
       <c r="B161" s="42">
         <f t="shared" si="10"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C161" s="42">
         <f t="shared" si="9"/>
-        <v>37744683.047763288</v>
+        <v>22012129.016454756</v>
       </c>
       <c r="D161" s="42">
         <f>SUM($C$2:C161)</f>
-        <v>5233282508.1802645</v>
+        <v>2058574397.6625631</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -7074,15 +7060,15 @@
       </c>
       <c r="B162" s="42">
         <f t="shared" si="10"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C162" s="42">
         <f t="shared" si="9"/>
-        <v>41915920.751829103</v>
+        <v>26222600.022344287</v>
       </c>
       <c r="D162" s="42">
         <f>SUM($C$2:C162)</f>
-        <v>5275198428.9320936</v>
+        <v>2084796997.6849074</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -7091,15 +7077,15 @@
       </c>
       <c r="B163" s="42">
         <f t="shared" ref="B163:B182" si="11">IF(A163=0,$N$42,0)+IF(A163=0,0,$O$42)+IF(MOD(A163,2)=0,$P$42,0)+IF(MOD(A163,3)=0,$Q$42,0)+IF(MOD(A163,6)=0,$R$42,0)+IF(MOD(A163,12)=0,$S$42,0)</f>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C163" s="42">
         <f t="shared" si="9"/>
-        <v>41811392.271151222</v>
+        <v>26157207.004832204</v>
       </c>
       <c r="D163" s="42">
         <f>SUM($C$2:C163)</f>
-        <v>5317009821.2032452</v>
+        <v>2110954204.6897397</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -7108,15 +7094,15 @@
       </c>
       <c r="B164" s="42">
         <f t="shared" si="11"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C164" s="42">
         <f t="shared" si="9"/>
-        <v>37463007.474951506</v>
+        <v>21847860.077127043</v>
       </c>
       <c r="D164" s="42">
         <f>SUM($C$2:C164)</f>
-        <v>5354472828.6781969</v>
+        <v>2132802064.7668667</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -7125,15 +7111,15 @@
       </c>
       <c r="B165" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C165" s="42">
         <f t="shared" si="9"/>
-        <v>41603116.668330409</v>
+        <v>26026909.787707504</v>
       </c>
       <c r="D165" s="42">
         <f>SUM($C$2:C165)</f>
-        <v>5396075945.3465271</v>
+        <v>2158828974.554574</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -7142,15 +7128,15 @@
       </c>
       <c r="B166" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C166" s="42">
         <f t="shared" si="9"/>
-        <v>41499368.247711122</v>
+        <v>25962004.775768079</v>
       </c>
       <c r="D166" s="42">
         <f>SUM($C$2:C166)</f>
-        <v>5437575313.5942383</v>
+        <v>2184790979.3303423</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -7159,15 +7145,15 @@
       </c>
       <c r="B167" s="42">
         <f t="shared" si="11"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C167" s="42">
         <f t="shared" si="9"/>
-        <v>37183433.949949168</v>
+        <v>21684817.020330168</v>
       </c>
       <c r="D167" s="42">
         <f>SUM($C$2:C167)</f>
-        <v>5474758747.5441875</v>
+        <v>2206475796.3506722</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -7176,15 +7162,15 @@
       </c>
       <c r="B168" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C168" s="42">
         <f t="shared" si="9"/>
-        <v>41292646.93399781</v>
+        <v>25832679.921909031</v>
       </c>
       <c r="D168" s="42">
         <f>SUM($C$2:C168)</f>
-        <v>5516051394.4781857</v>
+        <v>2232308476.2725811</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -7193,15 +7179,15 @@
       </c>
       <c r="B169" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C169" s="42">
         <f t="shared" ref="C169:C177" si="12">-PV($K$1,A169,,B169)</f>
-        <v>41189672.752117515</v>
+        <v>25768259.273724716</v>
       </c>
       <c r="D169" s="42">
         <f>SUM($C$2:C169)</f>
-        <v>5557241067.2303028</v>
+        <v>2258076735.5463057</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -7210,15 +7196,15 @@
       </c>
       <c r="B170" s="42">
         <f t="shared" si="11"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C170" s="42">
         <f t="shared" si="12"/>
-        <v>-22259268.937842578</v>
+        <v>-37642225.026014946</v>
       </c>
       <c r="D170" s="42">
         <f>SUM($C$2:C170)</f>
-        <v>5534981798.2924604</v>
+        <v>2220434510.5202909</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -7227,15 +7213,15 @@
       </c>
       <c r="B171" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C171" s="42">
         <f t="shared" si="12"/>
-        <v>40984494.12838728</v>
+        <v>25639899.526719082</v>
       </c>
       <c r="D171" s="42">
         <f>SUM($C$2:C171)</f>
-        <v>5575966292.4208479</v>
+        <v>2246074410.0470099</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -7244,15 +7230,15 @@
       </c>
       <c r="B172" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C172" s="42">
         <f t="shared" si="12"/>
-        <v>40882288.407368861</v>
+        <v>25575959.627649959</v>
       </c>
       <c r="D172" s="42">
         <f>SUM($C$2:C172)</f>
-        <v>5616848580.8282166</v>
+        <v>2271650369.6746597</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -7261,15 +7247,15 @@
       </c>
       <c r="B173" s="42">
         <f t="shared" si="11"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C173" s="42">
         <f t="shared" si="12"/>
-        <v>36630530.413002506</v>
+        <v>21362372.029243</v>
       </c>
       <c r="D173" s="42">
         <f>SUM($C$2:C173)</f>
-        <v>5653479111.2412195</v>
+        <v>2293012741.7039027</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -7278,15 +7264,15 @@
       </c>
       <c r="B174" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C174" s="42">
         <f t="shared" si="12"/>
-        <v>40678640.961057566</v>
+        <v>25448557.785237614</v>
       </c>
       <c r="D174" s="42">
         <f>SUM($C$2:C174)</f>
-        <v>5694157752.2022772</v>
+        <v>2318461299.4891405</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -7295,15 +7281,15 @@
       </c>
       <c r="B175" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C175" s="42">
         <f t="shared" si="12"/>
-        <v>40577197.966142207</v>
+        <v>25385095.047618564</v>
       </c>
       <c r="D175" s="42">
         <f>SUM($C$2:C175)</f>
-        <v>5734734950.1684198</v>
+        <v>2343846394.5367589</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -7312,15 +7298,15 @@
       </c>
       <c r="B176" s="42">
         <f t="shared" si="11"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C176" s="42">
         <f t="shared" si="12"/>
-        <v>36357169.377663426</v>
+        <v>21202952.002577499</v>
       </c>
       <c r="D176" s="42">
         <f>SUM($C$2:C176)</f>
-        <v>5771092119.5460835</v>
+        <v>2365049346.5393362</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -7329,15 +7315,15 @@
       </c>
       <c r="B177" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C177" s="42">
         <f t="shared" si="12"/>
-        <v>40375070.270600028</v>
+        <v>25258643.961287379</v>
       </c>
       <c r="D177" s="42">
         <f>SUM($C$2:C177)</f>
-        <v>5811467189.8166838</v>
+        <v>2390307990.5006237</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -7346,15 +7332,15 @@
       </c>
       <c r="B178" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C178" s="42">
         <f t="shared" ref="C178:C182" si="13">-PV($K$1,A178,,B178)</f>
-        <v>40274384.309825458</v>
+        <v>25195654.824226808</v>
       </c>
       <c r="D178" s="42">
         <f>SUM($C$2:C178)</f>
-        <v>5851741574.1265097</v>
+        <v>2415503645.3248506</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -7363,15 +7349,15 @@
       </c>
       <c r="B179" s="42">
         <f t="shared" si="11"/>
-        <v>56140000</v>
+        <v>32740000</v>
       </c>
       <c r="C179" s="42">
         <f t="shared" si="13"/>
-        <v>36085848.341603622</v>
+        <v>21044721.672677282</v>
       </c>
       <c r="D179" s="42">
         <f>SUM($C$2:C179)</f>
-        <v>5887827422.4681129</v>
+        <v>2436548366.9975281</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -7380,15 +7366,15 @@
       </c>
       <c r="B180" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C180" s="42">
         <f t="shared" si="13"/>
-        <v>40073765.023675688</v>
+        <v>25070147.398811508</v>
       </c>
       <c r="D180" s="42">
         <f>SUM($C$2:C180)</f>
-        <v>5927901187.4917889</v>
+        <v>2461618514.3963394</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -7397,15 +7383,15 @@
       </c>
       <c r="B181" s="42">
         <f t="shared" si="11"/>
-        <v>62500000</v>
+        <v>39100000</v>
       </c>
       <c r="C181" s="42">
         <f t="shared" si="13"/>
-        <v>39973830.447556801</v>
+        <v>25007628.327991534</v>
       </c>
       <c r="D181" s="42">
         <f>SUM($C$2:C181)</f>
-        <v>5967875017.9393454</v>
+        <v>2486626142.7243309</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -7414,15 +7400,15 @@
       </c>
       <c r="B182" s="42">
         <f t="shared" si="11"/>
-        <v>-33860000</v>
+        <v>-57260000</v>
       </c>
       <c r="C182" s="42">
         <f t="shared" si="13"/>
-        <v>-21602216.841165457</v>
+        <v>-36531096.760931313</v>
       </c>
       <c r="D182" s="42">
         <f>SUM($C$2:C182)</f>
-        <v>5946272801.0981798</v>
+        <v>2450095045.9633994</v>
       </c>
     </row>
   </sheetData>
@@ -7443,7 +7429,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="89.5703125" customWidth="1"/>
     <col min="2" max="1025" width="11.5703125"/>
@@ -7480,7 +7466,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>